<commit_message>
First working edition with WinPatcher. A little unstable on x64 release
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>TortureTest Windows XP on x64 quad-core (Intel 2.66Ghz Q6700)</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>SpeedTest Windows XP on x64 quad-core (Intel 2.66Ghz Q6700)</t>
+  </si>
+  <si>
+    <t>SpeedTest Windows XP on x86 quad-core (Intel 2.66Ghz Q6700)</t>
+  </si>
+  <si>
+    <t>TortureTest Windows XP on x86 quad-core (Intel 2.66Ghz Q6700)</t>
   </si>
 </sst>
 </file>
@@ -362,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -375,61 +381,12 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>515958</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>15630038</v>
-      </c>
-      <c r="G4">
-        <f>F4/F$3</f>
-        <v>30.29323704642626</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>698115</v>
-      </c>
-      <c r="G5">
-        <f>F5/F$3</f>
-        <v>1.3530461781772936</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -454,7 +411,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>373505</v>
+        <v>515958</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -462,11 +419,11 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>409623</v>
+        <v>15630038</v>
       </c>
       <c r="G13">
         <f>F13/F$12</f>
-        <v>1.096700178043132</v>
+        <v>30.29323704642626</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -474,10 +431,69 @@
         <v>3</v>
       </c>
       <c r="F14">
-        <v>396249</v>
+        <v>698115</v>
       </c>
       <c r="G14">
         <f>F14/F$12</f>
+        <v>1.3530461781772936</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>373505</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>409623</v>
+      </c>
+      <c r="G33">
+        <f>F33/F$32</f>
+        <v>1.096700178043132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>396249</v>
+      </c>
+      <c r="G34">
+        <f>F34/F$32</f>
         <v>1.0608934284681597</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed missing page execute segfault Added _msize support
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>TortureTest Windows XP on x64 quad-core (Intel 2.66Ghz Q6700)</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>TortureTest Windows XP on x86 quad-core (Intel 2.66Ghz Q6700)</t>
+  </si>
+  <si>
+    <t>nedmalloc v1.06 (threadcached sysalloc)</t>
+  </si>
+  <si>
+    <t>nedmalloc v1.06 (patcher)</t>
   </si>
 </sst>
 </file>
@@ -371,7 +377,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -384,6 +390,60 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:7">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>515958</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>31089140</v>
+      </c>
+      <c r="G4">
+        <f>F4/F$3</f>
+        <v>60.255175808883671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>30994083</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G6" si="0">F5/F$3</f>
+        <v>60.070941820845881</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>4</v>
@@ -411,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>515958</v>
+        <v>14491780</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -419,23 +479,28 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>15630038</v>
+        <v>37044111</v>
       </c>
       <c r="G13">
         <f>F13/F$12</f>
-        <v>30.29323704642626</v>
+        <v>2.556215385549601</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F14">
-        <v>698115</v>
+        <v>36643063</v>
       </c>
       <c r="G14">
         <f>F14/F$12</f>
-        <v>1.3530461781772936</v>
+        <v>2.5285412143987833</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6">

</xml_diff>

<commit_message>
Removed some cold code in GetThreadCache() and added some more RESTRICT qualifiers. Added LTCG optimisation for MSVC. Added first attempt at a SConstruct file for later TnFOX integration of the LTCG nedmalloc DLL.
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>TortureTest Windows XP on x64 quad-core (Intel 2.66Ghz Q6700)</t>
   </si>
@@ -43,6 +43,30 @@
   </si>
   <si>
     <t>nedmalloc v1.06 (patcher)</t>
+  </si>
+  <si>
+    <t>Win32 (low frag)</t>
+  </si>
+  <si>
+    <t>noinline, noforceinline</t>
+  </si>
+  <si>
+    <t>noforceinline</t>
+  </si>
+  <si>
+    <t>all enabled</t>
+  </si>
+  <si>
+    <t>noforceinline + LTCG</t>
+  </si>
+  <si>
+    <t>One thread, 10000 record SpeedTest x64:</t>
+  </si>
+  <si>
+    <t>Removed cold code from GetThreadCache</t>
+  </si>
+  <si>
+    <t>noforceinline, /O1</t>
   </si>
 </sst>
 </file>
@@ -374,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -409,7 +433,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>515958</v>
@@ -435,7 +459,7 @@
         <v>30994083</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G6" si="0">F5/F$3</f>
+        <f t="shared" ref="G5" si="0">F5/F$3</f>
         <v>60.070941820845881</v>
       </c>
     </row>
@@ -503,17 +527,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="21" spans="1:7">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>597722</v>
+      </c>
+      <c r="G23" t="e">
+        <f>F23/F$22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" t="e">
+        <f>F24/F$22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="B31">
         <v>1</v>
       </c>
@@ -530,7 +597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -542,28 +609,95 @@
       <c r="A33" t="s">
         <v>2</v>
       </c>
+      <c r="B33">
+        <v>626096</v>
+      </c>
       <c r="F33">
-        <v>409623</v>
+        <v>542544</v>
       </c>
       <c r="G33">
         <f>F33/F$32</f>
-        <v>1.096700178043132</v>
+        <v>1.4525749320624892</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="F34">
-        <v>396249</v>
-      </c>
       <c r="G34">
         <f>F34/F$32</f>
-        <v>1.0608934284681597</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>748133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>750395</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>749212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>742156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>753032</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>747830</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>746683</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added a small convenience patch for uthash
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>TortureTest Windows XP on x64 quad-core (Intel 2.66Ghz Q6700)</t>
   </si>
@@ -60,13 +60,37 @@
     <t>noforceinline + LTCG</t>
   </si>
   <si>
-    <t>One thread, 10000 record SpeedTest x64:</t>
-  </si>
-  <si>
     <t>Removed cold code from GetThreadCache</t>
   </si>
   <si>
     <t>noforceinline, /O1</t>
+  </si>
+  <si>
+    <t>One thread, 10000 record TortureTest x64:</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>LTCG off</t>
+  </si>
+  <si>
+    <t>/GS-</t>
+  </si>
+  <si>
+    <t>DLL, fast heap detect</t>
+  </si>
+  <si>
+    <t>static, fast heap detect</t>
+  </si>
+  <si>
+    <t>static, normal detect</t>
+  </si>
+  <si>
+    <t>DLL, normal detect</t>
+  </si>
+  <si>
+    <t>/GS-, SSE2</t>
   </si>
 </sst>
 </file>
@@ -398,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -631,7 +655,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -641,6 +665,9 @@
       <c r="B37">
         <v>748133</v>
       </c>
+      <c r="F37">
+        <v>648429</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
@@ -649,6 +676,9 @@
       <c r="B38">
         <v>750395</v>
       </c>
+      <c r="F38">
+        <v>658633</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
@@ -668,7 +698,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -689,10 +719,94 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B44">
         <v>746683</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45">
+        <v>779216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46">
+        <v>791479</v>
+      </c>
+      <c r="C46">
+        <f>(B46-B45)/B45</f>
+        <v>1.5737613190694236E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48">
+        <v>769324</v>
+      </c>
+      <c r="E48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48">
+        <v>807550</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49">
+        <v>784905</v>
+      </c>
+      <c r="C49">
+        <f>(B49-B48)/B48</f>
+        <v>2.0252845355142955E-2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49">
+        <v>796140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="E50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50">
+        <v>796782</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51">
+        <v>780550</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52">
+        <v>773581</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53">
+        <v>768500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>